<commit_message>
updated fubar results with corrected vp6a dataset
</commit_message>
<xml_diff>
--- a/20 Results/selectionhost.xlsx
+++ b/20 Results/selectionhost.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qx217\Documents\rotavirus\20 Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rotavirus\20 Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -263,15 +263,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -304,7 +304,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -400,6 +399,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FB63-4626-9E83-8F52BA028F44}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -460,6 +464,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FB63-4626-9E83-8F52BA028F44}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -591,7 +600,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -659,7 +667,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -673,7 +681,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -769,6 +776,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-109A-4BAC-A3A2-28E06D5C674D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -829,6 +841,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-109A-4BAC-A3A2-28E06D5C674D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -960,7 +977,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1028,7 +1044,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1042,7 +1058,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1138,6 +1153,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E26-47A8-8216-EBA2437E5189}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1198,6 +1218,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E26-47A8-8216-EBA2437E5189}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1329,7 +1354,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1397,7 +1421,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1411,7 +1435,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1519,6 +1542,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-51DB-4545-A43F-A0D40A86B67B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1591,6 +1619,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-51DB-4545-A43F-A0D40A86B67B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1663,6 +1696,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-51DB-4545-A43F-A0D40A86B67B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1794,7 +1832,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1862,7 +1899,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1876,7 +1913,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1990,6 +2026,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6004-4B21-B585-9B622527EBA3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2068,6 +2109,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6004-4B21-B585-9B622527EBA3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2146,6 +2192,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6004-4B21-B585-9B622527EBA3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2277,7 +2328,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2345,7 +2395,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2359,7 +2409,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG"/>
+              <a:t>Selection</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-SG" baseline="0"/>
+              <a:t> in RVB</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-SG"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2467,6 +2546,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7ADE-4774-885D-14A6A01C9432}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2539,6 +2623,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7ADE-4774-885D-14A6A01C9432}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2560,6 +2649,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG"/>
+                  <a:t>Proteins</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2625,6 +2769,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG"/>
+                  <a:t>dN/dS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2670,7 +2869,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2738,7 +2936,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2752,7 +2950,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG"/>
+              <a:t>Selection in RVC</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2866,6 +3088,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7279-46F6-ABE5-6AA37DB1B18C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2944,6 +3171,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7279-46F6-ABE5-6AA37DB1B18C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2965,6 +3197,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG"/>
+                  <a:t>Proteins</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3030,6 +3317,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG"/>
+                  <a:t>dN/dS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3075,7 +3417,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7137,14 +7478,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>128587</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>519112</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>433387</xdr:colOff>
+      <xdr:colOff>214312</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
@@ -7244,6 +7585,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -7279,6 +7637,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7718,12 +8093,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="F1" t="s">
         <v>25</v>
       </c>
@@ -7776,19 +8151,19 @@
       <c r="I3">
         <v>2.2715378976928598E-2</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -7817,19 +8192,19 @@
       <c r="I4">
         <v>3.0616358711997398E-2</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="S4" s="4">
+      <c r="S4" s="3">
         <v>3</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T4" s="3">
         <v>0.14390085431422159</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="3">
         <v>4.7966951438073863E-2</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="3">
         <v>1.4211836910648966E-3</v>
       </c>
     </row>
@@ -7846,19 +8221,19 @@
       <c r="D5">
         <v>2.90752645821509E-2</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5" s="3">
         <v>3</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T5" s="3">
         <v>0.19035118348117538</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5" s="3">
         <v>6.3450394493725124E-2</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5" s="3">
         <v>1.0740967508344234E-3</v>
       </c>
     </row>
@@ -7875,11 +8250,11 @@
       <c r="D6">
         <v>7.8243559586239797E-2</v>
       </c>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -7894,19 +8269,19 @@
       <c r="D7">
         <v>2.1304132056855801E-2</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="S7" s="4">
+      <c r="S7" s="3">
         <v>2</v>
       </c>
-      <c r="T7" s="4">
+      <c r="T7" s="3">
         <v>0.18746311642301489</v>
       </c>
-      <c r="U7" s="4">
+      <c r="U7" s="3">
         <v>9.3731558211507443E-2</v>
       </c>
-      <c r="V7" s="4">
+      <c r="V7" s="3">
         <v>1.1822369807437068E-5</v>
       </c>
     </row>
@@ -7923,36 +8298,36 @@
       <c r="D8">
         <v>3.09682684877715E-2</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="R8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="S8" s="4">
+      <c r="S8" s="3">
         <v>2</v>
       </c>
-      <c r="T8" s="4">
+      <c r="T8" s="3">
         <v>9.3457183683456097E-2</v>
       </c>
-      <c r="U8" s="4">
+      <c r="U8" s="3">
         <v>4.6728591841728048E-2</v>
       </c>
-      <c r="V8" s="4">
+      <c r="V8" s="3">
         <v>5.6739902562360969E-4</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R9" s="5" t="s">
+      <c r="R9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="S9" s="5">
+      <c r="S9" s="4">
         <v>2</v>
       </c>
-      <c r="T9" s="5">
+      <c r="T9" s="4">
         <v>5.3331737688925997E-2</v>
       </c>
-      <c r="U9" s="5">
+      <c r="U9" s="4">
         <v>2.6665868844462998E-2</v>
       </c>
-      <c r="V9" s="5">
+      <c r="V9" s="4">
         <v>3.1212740386984007E-5</v>
       </c>
     </row>
@@ -7962,48 +8337,48 @@
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="R13" s="6" t="s">
+      <c r="R13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="S13" s="6" t="s">
+      <c r="S13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="T13" s="6" t="s">
+      <c r="T13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="U13" s="6" t="s">
+      <c r="U13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="V13" s="6" t="s">
+      <c r="V13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="W13" s="6" t="s">
+      <c r="W13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="X13" s="6" t="s">
+      <c r="X13" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="R14" s="4" t="s">
+      <c r="R14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S14" s="4">
+      <c r="S14" s="3">
         <v>3.5960551328639498E-4</v>
       </c>
-      <c r="T14" s="4">
+      <c r="T14" s="3">
         <v>1</v>
       </c>
-      <c r="U14" s="4">
+      <c r="U14" s="3">
         <v>3.5960551328639498E-4</v>
       </c>
-      <c r="V14" s="4">
+      <c r="V14" s="3">
         <v>2.8673403350611646</v>
       </c>
-      <c r="W14" s="4">
+      <c r="W14" s="3">
         <v>0.23247281806545461</v>
       </c>
-      <c r="X14" s="4">
+      <c r="X14" s="3">
         <v>18.512820512820511</v>
       </c>
     </row>
@@ -8011,25 +8386,25 @@
       <c r="F15" t="s">
         <v>22</v>
       </c>
-      <c r="R15" s="4" t="s">
+      <c r="R15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="S15" s="4">
+      <c r="S15" s="3">
         <v>4.7397322612670011E-3</v>
       </c>
-      <c r="T15" s="4">
+      <c r="T15" s="3">
         <v>2</v>
       </c>
-      <c r="U15" s="4">
+      <c r="U15" s="3">
         <v>2.3698661306335005E-3</v>
       </c>
-      <c r="V15" s="4">
+      <c r="V15" s="3">
         <v>18.896297453729421</v>
       </c>
-      <c r="W15" s="4">
+      <c r="W15" s="3">
         <v>5.0260607649518084E-2</v>
       </c>
-      <c r="X15" s="4">
+      <c r="X15" s="3">
         <v>18.999999999999996</v>
       </c>
     </row>
@@ -8043,21 +8418,21 @@
       <c r="I16" t="s">
         <v>49</v>
       </c>
-      <c r="R16" s="4" t="s">
+      <c r="R16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S16" s="4">
+      <c r="S16" s="3">
         <v>2.5082862253163543E-4</v>
       </c>
-      <c r="T16" s="4">
+      <c r="T16" s="3">
         <v>2</v>
       </c>
-      <c r="U16" s="4">
+      <c r="U16" s="3">
         <v>1.2541431126581772E-4</v>
       </c>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
     </row>
     <row r="17" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
@@ -8072,13 +8447,13 @@
       <c r="I17">
         <v>3.5645046269771399E-2</v>
       </c>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
     </row>
     <row r="18" spans="6:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
@@ -8093,19 +8468,19 @@
       <c r="I18">
         <v>3.0551107291359202E-2</v>
       </c>
-      <c r="R18" s="5" t="s">
+      <c r="R18" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="S18" s="5">
+      <c r="S18" s="4">
         <v>5.3501663970850315E-3</v>
       </c>
-      <c r="T18" s="5">
+      <c r="T18" s="4">
         <v>5</v>
       </c>
-      <c r="U18" s="5"/>
-      <c r="V18" s="5"/>
-      <c r="W18" s="5"/>
-      <c r="X18" s="5"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
     </row>
     <row r="20" spans="6:24" x14ac:dyDescent="0.25">
       <c r="R20" t="s">
@@ -8114,77 +8489,77 @@
     </row>
     <row r="21" spans="6:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="R22" s="6" t="s">
+      <c r="R22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="S22" s="6" t="s">
+      <c r="S22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="T22" s="6" t="s">
+      <c r="T22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="U22" s="6" t="s">
+      <c r="U22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="V22" s="6" t="s">
+      <c r="V22" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="R23" s="4" t="s">
+      <c r="R23" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="S23" s="4">
+      <c r="S23" s="3">
         <v>3</v>
       </c>
-      <c r="T23" s="4">
+      <c r="T23" s="3">
         <v>0.13609061485298712</v>
       </c>
-      <c r="U23" s="4">
+      <c r="U23" s="3">
         <v>4.5363538284329041E-2</v>
       </c>
-      <c r="V23" s="4">
+      <c r="V23" s="3">
         <v>4.9988843804415041E-4</v>
       </c>
     </row>
     <row r="24" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="R24" s="4" t="s">
+      <c r="R24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="S24" s="4">
+      <c r="S24" s="3">
         <v>3</v>
       </c>
-      <c r="T24" s="4">
+      <c r="T24" s="3">
         <v>0.21395904619771111</v>
       </c>
-      <c r="U24" s="4">
+      <c r="U24" s="3">
         <v>7.1319682065903708E-2</v>
       </c>
-      <c r="V24" s="4">
+      <c r="V24" s="3">
         <v>1.4646098357805832E-3</v>
       </c>
     </row>
     <row r="25" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
     </row>
     <row r="26" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="R26" s="4" t="s">
+      <c r="R26" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="S26" s="4">
+      <c r="S26" s="3">
         <v>2</v>
       </c>
-      <c r="T26" s="4">
+      <c r="T26" s="3">
         <v>0.13597978711587219</v>
       </c>
-      <c r="U26" s="4">
+      <c r="U26" s="3">
         <v>6.7989893557936096E-2</v>
       </c>
-      <c r="V26" s="4">
+      <c r="V26" s="3">
         <v>2.9615240183235043E-3</v>
       </c>
     </row>
@@ -8192,19 +8567,19 @@
       <c r="F27" t="s">
         <v>23</v>
       </c>
-      <c r="R27" s="4" t="s">
+      <c r="R27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="S27" s="4">
+      <c r="S27" s="3">
         <v>2</v>
       </c>
-      <c r="T27" s="4">
+      <c r="T27" s="3">
         <v>0.14787372037369539</v>
       </c>
-      <c r="U27" s="4">
+      <c r="U27" s="3">
         <v>7.3936860186847697E-2</v>
       </c>
-      <c r="V27" s="4">
+      <c r="V27" s="3">
         <v>1.8006175371907361E-5</v>
       </c>
     </row>
@@ -8218,19 +8593,19 @@
       <c r="I28" t="s">
         <v>49</v>
       </c>
-      <c r="R28" s="5" t="s">
+      <c r="R28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="S28" s="5">
+      <c r="S28" s="4">
         <v>2</v>
       </c>
-      <c r="T28" s="5">
+      <c r="T28" s="4">
         <v>6.6196153561130594E-2</v>
       </c>
-      <c r="U28" s="5">
+      <c r="U28" s="4">
         <v>3.3098076780565297E-2</v>
       </c>
-      <c r="V28" s="5">
+      <c r="V28" s="4">
         <v>1.2974107157893552E-5</v>
       </c>
     </row>
@@ -8268,114 +8643,114 @@
       </c>
     </row>
     <row r="32" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="R32" s="6" t="s">
+      <c r="R32" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="S32" s="6" t="s">
+      <c r="S32" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="T32" s="6" t="s">
+      <c r="T32" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="U32" s="6" t="s">
+      <c r="U32" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="V32" s="6" t="s">
+      <c r="V32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="W32" s="6" t="s">
+      <c r="W32" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="X32" s="6" t="s">
+      <c r="X32" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="33" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R33" s="4" t="s">
+      <c r="R33" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S33" s="4">
+      <c r="S33" s="3">
         <v>1.0105821000146653E-3</v>
       </c>
-      <c r="T33" s="4">
+      <c r="T33" s="3">
         <v>1</v>
       </c>
-      <c r="U33" s="4">
+      <c r="U33" s="3">
         <v>1.0105821000146653E-3</v>
       </c>
-      <c r="V33" s="4">
+      <c r="V33" s="3">
         <v>1.0197999695316433</v>
       </c>
-      <c r="W33" s="4">
+      <c r="W33" s="3">
         <v>0.41887653888489762</v>
       </c>
-      <c r="X33" s="4">
+      <c r="X33" s="3">
         <v>18.512820512820511</v>
       </c>
     </row>
     <row r="34" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R34" s="4" t="s">
+      <c r="R34" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="S34" s="4">
+      <c r="S34" s="3">
         <v>1.9470743468108327E-3</v>
       </c>
-      <c r="T34" s="4">
+      <c r="T34" s="3">
         <v>2</v>
       </c>
-      <c r="U34" s="4">
+      <c r="U34" s="3">
         <v>9.7353717340541634E-4</v>
       </c>
-      <c r="V34" s="4">
+      <c r="V34" s="3">
         <v>0.98241714331013619</v>
       </c>
-      <c r="W34" s="4">
+      <c r="W34" s="3">
         <v>0.50443470153322645</v>
       </c>
-      <c r="X34" s="4">
+      <c r="X34" s="3">
         <v>18.999999999999996</v>
       </c>
     </row>
     <row r="35" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R35" s="4" t="s">
+      <c r="R35" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S35" s="4">
+      <c r="S35" s="3">
         <v>1.9819222008386379E-3</v>
       </c>
-      <c r="T35" s="4">
+      <c r="T35" s="3">
         <v>2</v>
       </c>
-      <c r="U35" s="4">
+      <c r="U35" s="3">
         <v>9.9096110041931897E-4</v>
       </c>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
     </row>
     <row r="36" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
-      <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
     </row>
     <row r="37" spans="18:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R37" s="5" t="s">
+      <c r="R37" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="S37" s="5">
+      <c r="S37" s="4">
         <v>4.9395786476641359E-3</v>
       </c>
-      <c r="T37" s="5">
+      <c r="T37" s="4">
         <v>5</v>
       </c>
-      <c r="U37" s="5"/>
-      <c r="V37" s="5"/>
-      <c r="W37" s="5"/>
-      <c r="X37" s="5"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
     </row>
     <row r="39" spans="18:24" x14ac:dyDescent="0.25">
       <c r="R39" t="s">
@@ -8384,111 +8759,111 @@
     </row>
     <row r="40" spans="18:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R41" s="6" t="s">
+      <c r="R41" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="S41" s="6" t="s">
+      <c r="S41" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="T41" s="6" t="s">
+      <c r="T41" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="U41" s="6" t="s">
+      <c r="U41" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="V41" s="6" t="s">
+      <c r="V41" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="42" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R42" s="4" t="s">
+      <c r="R42" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="S42" s="4">
+      <c r="S42" s="3">
         <v>3</v>
       </c>
-      <c r="T42" s="4">
+      <c r="T42" s="3">
         <v>0.1329400889214698</v>
       </c>
-      <c r="U42" s="4">
+      <c r="U42" s="3">
         <v>4.4313362973823267E-2</v>
       </c>
-      <c r="V42" s="4">
+      <c r="V42" s="3">
         <v>1.1122412746140797E-3</v>
       </c>
     </row>
     <row r="43" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R43" s="4" t="s">
+      <c r="R43" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="S43" s="4">
+      <c r="S43" s="3">
         <v>3</v>
       </c>
-      <c r="T43" s="4">
+      <c r="T43" s="3">
         <v>0.22599135085518729</v>
       </c>
-      <c r="U43" s="4">
+      <c r="U43" s="3">
         <v>7.5330450285062425E-2</v>
       </c>
-      <c r="V43" s="4">
+      <c r="V43" s="3">
         <v>1.8472574952022869E-3</v>
       </c>
     </row>
     <row r="44" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
-      <c r="T44" s="4"/>
-      <c r="U44" s="4"/>
-      <c r="V44" s="4"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+      <c r="V44" s="3"/>
     </row>
     <row r="45" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R45" s="4" t="s">
+      <c r="R45" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="S45" s="4">
+      <c r="S45" s="3">
         <v>2</v>
       </c>
-      <c r="T45" s="4">
+      <c r="T45" s="3">
         <v>0.19934021506363908</v>
       </c>
-      <c r="U45" s="4">
+      <c r="U45" s="3">
         <v>9.9670107531819541E-2</v>
       </c>
-      <c r="V45" s="4">
+      <c r="V45" s="3">
         <v>5.854641803498227E-4</v>
       </c>
     </row>
     <row r="46" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R46" s="4" t="s">
+      <c r="R46" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="S46" s="4">
+      <c r="S46" s="3">
         <v>2</v>
       </c>
-      <c r="T46" s="4">
+      <c r="T46" s="3">
         <v>0.1073188241683907</v>
       </c>
-      <c r="U46" s="4">
+      <c r="U46" s="3">
         <v>5.3659412084195349E-2</v>
       </c>
-      <c r="V46" s="4">
+      <c r="V46" s="3">
         <v>1.2087606168045568E-3</v>
       </c>
     </row>
     <row r="47" spans="18:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R47" s="5" t="s">
+      <c r="R47" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="S47" s="5">
+      <c r="S47" s="4">
         <v>2</v>
       </c>
-      <c r="T47" s="5">
+      <c r="T47" s="4">
         <v>5.2272400544627298E-2</v>
       </c>
-      <c r="U47" s="5">
+      <c r="U47" s="4">
         <v>2.6136200272313649E-2</v>
       </c>
-      <c r="V47" s="5">
+      <c r="V47" s="4">
         <v>4.6697766477676308E-5</v>
       </c>
     </row>
@@ -8498,114 +8873,114 @@
       </c>
     </row>
     <row r="51" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R51" s="6" t="s">
+      <c r="R51" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="S51" s="6" t="s">
+      <c r="S51" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="T51" s="6" t="s">
+      <c r="T51" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="U51" s="6" t="s">
+      <c r="U51" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="V51" s="6" t="s">
+      <c r="V51" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="W51" s="6" t="s">
+      <c r="W51" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="X51" s="6" t="s">
+      <c r="X51" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="52" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R52" s="4" t="s">
+      <c r="R52" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S52" s="4">
+      <c r="S52" s="3">
         <v>1.4430895579095491E-3</v>
       </c>
-      <c r="T52" s="4">
+      <c r="T52" s="3">
         <v>1</v>
       </c>
-      <c r="U52" s="4">
+      <c r="U52" s="3">
         <v>1.4430895579095491E-3</v>
       </c>
-      <c r="V52" s="4">
+      <c r="V52" s="3">
         <v>7.2547502954851559</v>
       </c>
-      <c r="W52" s="4">
+      <c r="W52" s="3">
         <v>0.11462168332043965</v>
       </c>
-      <c r="X52" s="4">
+      <c r="X52" s="3">
         <v>18.512820512820511</v>
       </c>
     </row>
     <row r="53" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R53" s="4" t="s">
+      <c r="R53" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="S53" s="4">
+      <c r="S53" s="3">
         <v>5.5211645339102288E-3</v>
       </c>
-      <c r="T53" s="4">
+      <c r="T53" s="3">
         <v>2</v>
       </c>
-      <c r="U53" s="4">
+      <c r="U53" s="3">
         <v>2.7605822669551144E-3</v>
       </c>
-      <c r="V53" s="4">
+      <c r="V53" s="3">
         <v>13.878095719793839</v>
       </c>
-      <c r="W53" s="4">
+      <c r="W53" s="3">
         <v>6.7212902701627247E-2</v>
       </c>
-      <c r="X53" s="4">
+      <c r="X53" s="3">
         <v>18.999999999999996</v>
       </c>
     </row>
     <row r="54" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R54" s="4" t="s">
+      <c r="R54" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S54" s="4">
+      <c r="S54" s="3">
         <v>3.9783300572250602E-4</v>
       </c>
-      <c r="T54" s="4">
+      <c r="T54" s="3">
         <v>2</v>
       </c>
-      <c r="U54" s="4">
+      <c r="U54" s="3">
         <v>1.9891650286125301E-4</v>
       </c>
-      <c r="V54" s="4"/>
-      <c r="W54" s="4"/>
-      <c r="X54" s="4"/>
+      <c r="V54" s="3"/>
+      <c r="W54" s="3"/>
+      <c r="X54" s="3"/>
     </row>
     <row r="55" spans="18:24" x14ac:dyDescent="0.25">
-      <c r="R55" s="4"/>
-      <c r="S55" s="4"/>
-      <c r="T55" s="4"/>
-      <c r="U55" s="4"/>
-      <c r="V55" s="4"/>
-      <c r="W55" s="4"/>
-      <c r="X55" s="4"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="3"/>
+      <c r="U55" s="3"/>
+      <c r="V55" s="3"/>
+      <c r="W55" s="3"/>
+      <c r="X55" s="3"/>
     </row>
     <row r="56" spans="18:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R56" s="5" t="s">
+      <c r="R56" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="S56" s="5">
+      <c r="S56" s="4">
         <v>7.3620870975422839E-3</v>
       </c>
-      <c r="T56" s="5">
+      <c r="T56" s="4">
         <v>5</v>
       </c>
-      <c r="U56" s="5"/>
-      <c r="V56" s="5"/>
-      <c r="W56" s="5"/>
-      <c r="X56" s="5"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4"/>
+      <c r="W56" s="4"/>
+      <c r="X56" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8620,19 +8995,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="F1" t="s">
         <v>27</v>
       </c>
@@ -8664,34 +9039,34 @@
       <c r="D3">
         <v>8.25606922824631E-2</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -8708,34 +9083,34 @@
       <c r="D4">
         <v>2.90752645821509E-2</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>3</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>0.20337018061438819</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>6.7790060204796068E-2</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>1.1181619091628903E-3</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="3">
         <v>3</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="3">
         <v>0.31941293798813797</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <v>0.10647097932937932</v>
       </c>
-      <c r="R4" s="4">
+      <c r="R4" s="3">
         <v>1.0626178836815902E-4</v>
       </c>
     </row>
@@ -8752,39 +9127,39 @@
       <c r="D5">
         <v>7.8852876369858493E-2</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>3</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>0.12989682017073451</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>4.3298940056911504E-2</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>5.7303364243880845E-4</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="3">
         <v>3</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="3">
         <v>0.21875290805480768</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <v>7.2917636018269227E-2</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5" s="3">
         <v>6.5932582665781039E-5</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B6">
@@ -8796,34 +9171,34 @@
       <c r="D6">
         <v>2.1304132056855801E-2</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>3</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>0.2851346621987591</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>9.5044887399586372E-2</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>6.9478911567008757E-4</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="3">
         <v>3</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="3">
         <v>0.36336653624040399</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
         <v>0.12112217874680133</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="3">
         <v>3.7656623274614706E-4</v>
       </c>
     </row>
@@ -8840,66 +9215,66 @@
       <c r="D7">
         <v>5.6436511687720001E-2</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>3</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>7.9664557303555802E-2</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>2.6554852434518602E-2</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>6.2471622439204486E-5</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="3">
         <v>3</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="3">
         <v>0.17449867930307039</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <v>5.8166226434356795E-2</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7" s="3">
         <v>3.6414721847896885E-4</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>3</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>0.1979954070635479</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>6.5998469021182629E-2</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <v>2.2771377653553037E-4</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="3">
         <v>3</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8" s="3">
         <v>0.20187187911779308</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8" s="3">
         <v>6.7290626372597695E-2</v>
       </c>
-      <c r="R8" s="4">
+      <c r="R8" s="3">
         <v>2.1904371858365128E-4</v>
       </c>
     </row>
@@ -8913,24 +9288,24 @@
       <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="N9" s="4" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="N9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="3">
         <v>3</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="3">
         <v>9.2135734491128093E-2</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <v>3.0711911497042697E-2</v>
       </c>
-      <c r="R9" s="4">
+      <c r="R9" s="3">
         <v>5.0353616995470388E-8</v>
       </c>
     </row>
@@ -8947,26 +9322,26 @@
       <c r="D10">
         <v>0.116779522781176</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>5</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>0.28288675866484919</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>5.6577351732969836E-2</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <v>9.1377098878111466E-4</v>
       </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -8981,39 +9356,39 @@
       <c r="D11">
         <v>7.8243559586239797E-2</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>5</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>0.34494539170708804</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>6.8989078341417612E-2</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <v>1.5176961340708627E-3</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="N11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11" s="3">
         <v>6</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11" s="3">
         <v>0.43389388551588409</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <v>7.2315647585980677E-2</v>
       </c>
-      <c r="R11" s="4">
+      <c r="R11" s="3">
         <v>1.6922632104508881E-3</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B12">
@@ -9025,34 +9400,34 @@
       <c r="D12">
         <v>0.11523972766448599</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>5</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="4">
         <v>0.26822947697904831</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="4">
         <v>5.3645895395809662E-2</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="4">
         <v>7.8223761564129345E-4</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="N12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O12" s="4">
+      <c r="O12" s="3">
         <v>6</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12" s="3">
         <v>0.4827853956647512</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12" s="3">
         <v>8.0464232610791872E-2</v>
       </c>
-      <c r="R12" s="4">
+      <c r="R12" s="3">
         <v>7.6319616959276274E-4</v>
       </c>
     </row>
@@ -9069,19 +9444,19 @@
       <c r="D13">
         <v>5.3625634320866603E-2</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="4">
         <v>6</v>
       </c>
-      <c r="P13" s="5">
+      <c r="P13" s="4">
         <v>0.45335939401470599</v>
       </c>
-      <c r="Q13" s="5">
+      <c r="Q13" s="4">
         <v>7.5559899002450998E-2</v>
       </c>
-      <c r="R13" s="5">
+      <c r="R13" s="4">
         <v>1.2082444760716251E-3</v>
       </c>
     </row>
@@ -9117,25 +9492,25 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="K16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L16" s="6" t="s">
+      <c r="L16" s="5" t="s">
         <v>40</v>
       </c>
       <c r="N16" t="s">
@@ -9143,193 +9518,193 @@
       </c>
     </row>
     <row r="17" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>8.1659082490832501E-3</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <v>4</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="3">
         <v>2.0414770622708125E-3</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="3">
         <v>3.4830726209255438</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="3">
         <v>6.2682384620088183E-2</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="3">
         <v>3.8378533545558975</v>
       </c>
-      <c r="N17" s="6" t="s">
+      <c r="N17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="O17" s="6" t="s">
+      <c r="O17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="P17" s="6" t="s">
+      <c r="P17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Q17" s="6" t="s">
+      <c r="Q17" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="R17" s="6" t="s">
+      <c r="R17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="S17" s="6" t="s">
+      <c r="S17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="T17" s="6" t="s">
+      <c r="T17" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>6.6342942760320121E-4</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <v>2</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="3">
         <v>3.3171471380160061E-4</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="3">
         <v>0.56595612018061447</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="3">
         <v>0.58899693017207211</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="3">
         <v>4.4589701075245118</v>
       </c>
-      <c r="N18" s="4" t="s">
+      <c r="N18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O18" s="4">
+      <c r="O18" s="3">
         <v>1.6256469678260478E-2</v>
       </c>
-      <c r="P18" s="4">
+      <c r="P18" s="3">
         <v>5</v>
       </c>
-      <c r="Q18" s="4">
+      <c r="Q18" s="3">
         <v>3.2512939356520955E-3</v>
       </c>
-      <c r="R18" s="4">
+      <c r="R18" s="3">
         <v>15.767292561733457</v>
       </c>
-      <c r="S18" s="4">
+      <c r="S18" s="3">
         <v>1.8291150583562166E-4</v>
       </c>
-      <c r="T18" s="4">
+      <c r="T18" s="3">
         <v>3.325834530413013</v>
       </c>
     </row>
     <row r="19" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>4.6889107048898419E-3</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="3">
         <v>8</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="3">
         <v>5.8611383811123024E-4</v>
       </c>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="N19" s="4" t="s">
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="N19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O19" s="4">
+      <c r="O19" s="3">
         <v>2.0195418660349726E-4</v>
       </c>
-      <c r="P19" s="4">
+      <c r="P19" s="3">
         <v>2</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="Q19" s="3">
         <v>1.0097709330174863E-4</v>
       </c>
-      <c r="R19" s="4">
+      <c r="R19" s="3">
         <v>0.48969284341337171</v>
       </c>
-      <c r="S19" s="4">
+      <c r="S19" s="3">
         <v>0.62677229778942123</v>
       </c>
-      <c r="T19" s="4">
+      <c r="T19" s="3">
         <v>4.1028210151304032</v>
       </c>
     </row>
     <row r="20" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="N20" s="4" t="s">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="N20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O20" s="4">
+      <c r="O20" s="3">
         <v>2.0620496023159018E-3</v>
       </c>
-      <c r="P20" s="4">
+      <c r="P20" s="3">
         <v>10</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="Q20" s="3">
         <v>2.0620496023159018E-4</v>
       </c>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
     </row>
     <row r="21" spans="6:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <v>1.3518248381576293E-2</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="4">
         <v>14</v>
       </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
     </row>
     <row r="45" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
     </row>
     <row r="46" spans="6:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G46" s="4">
         <v>1.8520473467179877E-2</v>
       </c>
-      <c r="H46" s="5">
+      <c r="H46" s="4">
         <v>17</v>
       </c>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9344,19 +9719,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" t="s">
         <v>27</v>
       </c>
@@ -9382,34 +9757,34 @@
       <c r="C3">
         <v>8.25606922824631E-2</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -9423,34 +9798,34 @@
       <c r="C4">
         <v>2.90752645821509E-2</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>2</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>0.11206991524902629</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>5.6034957624513146E-2</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>1.4072291982879358E-3</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>2</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="3">
         <v>0.22325008693048498</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="3">
         <v>0.11162504346524249</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <v>5.3137314036772528E-5</v>
       </c>
     </row>
@@ -9464,39 +9839,39 @@
       <c r="C5">
         <v>7.8852876369858493E-2</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>0.10001161019880341</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>5.0005805099401703E-2</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>8.7617505268855478E-4</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="3">
         <v>2</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="3">
         <v>0.1551809343432827</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="3">
         <v>7.759046717164135E-2</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <v>8.5305940401205905E-7</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B6">
@@ -9505,34 +9880,34 @@
       <c r="C6">
         <v>2.1304132056855801E-2</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>2</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>0.20431311514793049</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>0.10215655757396525</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>1.086123115325275E-3</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <v>2</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="3">
         <v>0.220578447450583</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="3">
         <v>0.1102892237252915</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
         <v>4.9014978503960423E-5</v>
       </c>
     </row>
@@ -9546,66 +9921,66 @@
       <c r="C7">
         <v>5.6436511687720001E-2</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>2</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>5.6949178326627201E-2</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>2.84745891633136E-2</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>1.0283091023110223E-4</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="3">
         <v>2</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="3">
         <v>0.1327352520541385</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="3">
         <v>6.6367626027069249E-2</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <v>3.2471670528187377E-4</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>2</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>0.13983104976374888</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>6.9915524881874441E-2</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>3.6336759337638261E-4</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8" s="3">
         <v>2</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="3">
         <v>0.14288069312183729</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8" s="3">
         <v>7.1440346560918647E-2</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8" s="3">
         <v>3.3476637131914927E-4</v>
       </c>
     </row>
@@ -9616,24 +9991,24 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="M9" s="4" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="M9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="3">
         <v>2</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="3">
         <v>6.1519375779130706E-2</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="3">
         <v>3.0759687889565353E-2</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <v>8.7011731896070294E-8</v>
       </c>
     </row>
@@ -9647,26 +10022,26 @@
       <c r="C10">
         <v>0.116779522781176</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>5</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>0.34494539170708804</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>6.8989078341417612E-2</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>1.5176961340708627E-3</v>
       </c>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -9678,34 +10053,34 @@
       <c r="C11">
         <v>7.8243559586239797E-2</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>5</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>0.26822947697904831</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>5.3645895395809662E-2</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>7.8223761564129345E-4</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="3">
         <v>6</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11" s="3">
         <v>0.4827853956647512</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11" s="3">
         <v>8.0464232610791872E-2</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <v>7.6319616959276274E-4</v>
       </c>
     </row>
@@ -9719,24 +10094,24 @@
       <c r="C12">
         <v>0.11523972766448599</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="M12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="4">
         <v>6</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="4">
         <v>0.45335939401470599</v>
       </c>
-      <c r="P12" s="5">
+      <c r="P12" s="4">
         <v>7.5559899002450998E-2</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="Q12" s="4">
         <v>1.2082444760716251E-3</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B13">
@@ -9770,25 +10145,25 @@
       <c r="C15">
         <v>3.09682684877715E-2</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="K15" s="5" t="s">
         <v>40</v>
       </c>
       <c r="M15" t="s">
@@ -9796,191 +10171,191 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>5.952542286195372E-3</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>4</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <v>1.488135571548843E-3</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="3">
         <v>1.833134899262441</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="3">
         <v>0.28580631361312619</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="3">
         <v>6.38823290869587</v>
       </c>
-      <c r="M16" s="6" t="s">
+      <c r="M16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="N16" s="6" t="s">
+      <c r="N16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="O16" s="6" t="s">
+      <c r="O16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="P16" s="6" t="s">
+      <c r="P16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="Q16" s="6" t="s">
+      <c r="Q16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="R16" s="6" t="s">
+      <c r="R16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="S16" s="6" t="s">
+      <c r="S16" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>5.8853315725598473E-4</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>1</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <v>5.8853315725598473E-4</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="3">
         <v>0.72497472042562894</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="3">
         <v>0.4424897533948593</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="3">
         <v>7.708647422176786</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N17" s="4">
+      <c r="N17" s="3">
         <v>9.1667852524699774E-3</v>
       </c>
-      <c r="O17" s="4">
+      <c r="O17" s="3">
         <v>5</v>
       </c>
-      <c r="P17" s="4">
+      <c r="P17" s="3">
         <v>1.8333570504939956E-3</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="Q17" s="3">
         <v>13.277153221797809</v>
       </c>
-      <c r="R17" s="4">
+      <c r="R17" s="3">
         <v>6.531301098878152E-3</v>
       </c>
-      <c r="S17" s="4">
+      <c r="S17" s="3">
         <v>5.0503290576326485</v>
       </c>
     </row>
     <row r="18" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>3.2471927126532631E-3</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>4</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <v>8.1179817816331577E-4</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="M18" s="4" t="s">
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="M18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="N18" s="4">
+      <c r="N18" s="3">
         <v>7.2157464425704268E-5</v>
       </c>
-      <c r="O18" s="4">
+      <c r="O18" s="3">
         <v>1</v>
       </c>
-      <c r="P18" s="4">
+      <c r="P18" s="3">
         <v>7.2157464425704268E-5</v>
       </c>
-      <c r="Q18" s="4">
+      <c r="Q18" s="3">
         <v>0.52256362775508247</v>
       </c>
-      <c r="R18" s="4">
+      <c r="R18" s="3">
         <v>0.50213857973130982</v>
       </c>
-      <c r="S18" s="4">
+      <c r="S18" s="3">
         <v>6.607890973703368</v>
       </c>
     </row>
     <row r="19" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="M19" s="4" t="s">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N19" s="4">
+      <c r="N19" s="3">
         <v>6.9041797585196046E-4</v>
       </c>
-      <c r="O19" s="4">
+      <c r="O19" s="3">
         <v>5</v>
       </c>
-      <c r="P19" s="4">
+      <c r="P19" s="3">
         <v>1.3808359517039208E-4</v>
       </c>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
     </row>
     <row r="20" spans="5:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <v>9.7882681561046198E-3</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <v>9</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
     </row>
     <row r="21" spans="5:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M21" s="5" t="s">
+      <c r="M21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="N21" s="5">
+      <c r="N21" s="4">
         <v>9.9293606927476422E-3</v>
       </c>
-      <c r="O21" s="5">
+      <c r="O21" s="4">
         <v>11</v>
       </c>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>